<commit_message>
Added result based on random generated dataset
</commit_message>
<xml_diff>
--- a/Test with manipulated Dataset/ProcessedData.xlsx
+++ b/Test with manipulated Dataset/ProcessedData.xlsx
@@ -534,7 +534,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Good marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -544,12 +544,12 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -629,22 +629,22 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Good marks in Computer Networks</t>
+          <t>Average marks in Computer Networks</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -709,7 +709,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -719,7 +719,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -729,17 +729,17 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -814,22 +814,22 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Average marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -909,27 +909,27 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
@@ -994,7 +994,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -1004,7 +1004,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
@@ -1014,7 +1014,7 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
@@ -1089,7 +1089,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -1099,22 +1099,22 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Good marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1184,7 +1184,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1194,27 +1194,27 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Good marks in Computer Networks</t>
+          <t>Average marks in Computer Networks</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
@@ -1279,7 +1279,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1299,17 +1299,17 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Poor marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
@@ -1374,7 +1374,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -1384,12 +1384,12 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1404,7 +1404,7 @@
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
@@ -1479,27 +1479,27 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>Poor marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Poor marks in Computer Networks</t>
+          <t>Average marks in Computer Networks</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Poor marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>Poor marks in Operation Research</t>
+          <t>Good marks in Operation Research</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
@@ -1564,7 +1564,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Average marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
@@ -1574,27 +1574,27 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Good marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
@@ -1669,27 +1669,27 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
@@ -1754,7 +1754,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -1764,27 +1764,27 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Good marks in Computer Networks</t>
+          <t>Average marks in Computer Networks</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S15" t="inlineStr">
@@ -1859,7 +1859,7 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Good marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -1874,12 +1874,12 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
@@ -1954,27 +1954,27 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
@@ -2039,7 +2039,7 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Average marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -2059,17 +2059,17 @@
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S18" t="inlineStr">
@@ -2134,7 +2134,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
@@ -2144,12 +2144,12 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Good marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2159,12 +2159,12 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Good marks in Operation Research</t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
@@ -2239,12 +2239,12 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2344,12 +2344,12 @@
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2429,7 +2429,7 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Good marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
@@ -2449,7 +2449,7 @@
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S22" t="inlineStr">
@@ -2514,7 +2514,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
@@ -2524,17 +2524,17 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
@@ -2544,7 +2544,7 @@
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S23" t="inlineStr">
@@ -2619,7 +2619,7 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
@@ -2704,7 +2704,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
@@ -2714,7 +2714,7 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
@@ -2729,12 +2729,12 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S25" t="inlineStr">
@@ -2799,7 +2799,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
@@ -2819,12 +2819,12 @@
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2904,7 +2904,7 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
@@ -2919,12 +2919,12 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S27" t="inlineStr">
@@ -2989,7 +2989,7 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
@@ -3009,17 +3009,17 @@
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>Poor marks in Operation Research</t>
+          <t>Good marks in Operation Research</t>
         </is>
       </c>
       <c r="S28" t="inlineStr">
@@ -3094,22 +3094,22 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -3179,7 +3179,7 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
@@ -3189,17 +3189,17 @@
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
@@ -3209,7 +3209,7 @@
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S30" t="inlineStr">
@@ -3284,12 +3284,12 @@
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3379,17 +3379,17 @@
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
@@ -3399,7 +3399,7 @@
       </c>
       <c r="R32" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S32" t="inlineStr">
@@ -3474,12 +3474,12 @@
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -3494,7 +3494,7 @@
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S33" t="inlineStr">
@@ -3559,7 +3559,7 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
@@ -3569,7 +3569,7 @@
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Good marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O34" t="inlineStr">
@@ -3579,12 +3579,12 @@
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -3654,7 +3654,7 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
@@ -3664,12 +3664,12 @@
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3679,7 +3679,7 @@
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
@@ -3759,7 +3759,7 @@
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O36" t="inlineStr">
@@ -3769,17 +3769,17 @@
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Poor marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
         <is>
-          <t>Poor marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S36" t="inlineStr">
@@ -3844,7 +3844,7 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
@@ -3854,12 +3854,12 @@
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3869,12 +3869,12 @@
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S37" t="inlineStr">
@@ -3939,7 +3939,7 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Average marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
@@ -3949,7 +3949,7 @@
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
@@ -3959,12 +3959,12 @@
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
@@ -4044,7 +4044,7 @@
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O39" t="inlineStr">
@@ -4054,17 +4054,17 @@
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S39" t="inlineStr">
@@ -4139,27 +4139,27 @@
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S40" t="inlineStr">
@@ -4224,7 +4224,7 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Poor marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
@@ -4234,7 +4234,7 @@
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O41" t="inlineStr">
@@ -4244,12 +4244,12 @@
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
@@ -4319,7 +4319,7 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
@@ -4329,12 +4329,12 @@
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -4349,7 +4349,7 @@
       </c>
       <c r="R42" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S42" t="inlineStr">
@@ -4414,7 +4414,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
@@ -4424,12 +4424,12 @@
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Good marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Poor marks in Computer Networks</t>
+          <t>Average marks in Computer Networks</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -4439,12 +4439,12 @@
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R43" t="inlineStr">
         <is>
-          <t>Poor marks in Operation Research</t>
+          <t>Good marks in Operation Research</t>
         </is>
       </c>
       <c r="S43" t="inlineStr">
@@ -4509,7 +4509,7 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
@@ -4529,12 +4529,12 @@
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
@@ -4604,7 +4604,7 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
@@ -4614,17 +4614,17 @@
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q45" t="inlineStr">
@@ -4634,7 +4634,7 @@
       </c>
       <c r="R45" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S45" t="inlineStr">
@@ -4709,27 +4709,27 @@
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Good marks in Operation Research</t>
         </is>
       </c>
       <c r="S46" t="inlineStr">
@@ -4814,7 +4814,7 @@
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q47" t="inlineStr">
@@ -4889,7 +4889,7 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
@@ -4899,27 +4899,27 @@
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Poor marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R48" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S48" t="inlineStr">
@@ -4984,7 +4984,7 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
@@ -4994,17 +4994,17 @@
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q49" t="inlineStr">
@@ -5079,7 +5079,7 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
@@ -5094,7 +5094,7 @@
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -5104,12 +5104,12 @@
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R50" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S50" t="inlineStr">
@@ -5184,7 +5184,7 @@
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Good marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O51" t="inlineStr">
@@ -5199,12 +5199,12 @@
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R51" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Good marks in Operation Research</t>
         </is>
       </c>
       <c r="S51" t="inlineStr">
@@ -5269,7 +5269,7 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Poor marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
@@ -5279,12 +5279,12 @@
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -5294,12 +5294,12 @@
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R52" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Good marks in Operation Research</t>
         </is>
       </c>
       <c r="S52" t="inlineStr">
@@ -5364,7 +5364,7 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
@@ -5384,7 +5384,7 @@
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q53" t="inlineStr">
@@ -5394,7 +5394,7 @@
       </c>
       <c r="R53" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S53" t="inlineStr">
@@ -5469,27 +5469,27 @@
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R54" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S54" t="inlineStr">
@@ -5554,7 +5554,7 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M55" t="inlineStr">
@@ -5569,7 +5569,7 @@
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -5579,7 +5579,7 @@
       </c>
       <c r="Q55" t="inlineStr">
         <is>
-          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R55" t="inlineStr">
@@ -5659,27 +5659,27 @@
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q56" t="inlineStr">
         <is>
-          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R56" t="inlineStr">
         <is>
-          <t>Poor marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S56" t="inlineStr">
@@ -5744,7 +5744,7 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M57" t="inlineStr">
@@ -5759,7 +5759,7 @@
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Good marks in Computer Networks</t>
+          <t>Average marks in Computer Networks</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -5769,12 +5769,12 @@
       </c>
       <c r="Q57" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R57" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S57" t="inlineStr">
@@ -5859,17 +5859,17 @@
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R58" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S58" t="inlineStr">
@@ -5934,7 +5934,7 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M59" t="inlineStr">
@@ -5944,27 +5944,27 @@
       </c>
       <c r="N59" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Good marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R59" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S59" t="inlineStr">
@@ -6039,22 +6039,22 @@
       </c>
       <c r="N60" t="inlineStr">
         <is>
-          <t>Poor marks in Data Base Management System</t>
+          <t>Good marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Poor marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Poor marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R60" t="inlineStr">
@@ -6124,7 +6124,7 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M61" t="inlineStr">
@@ -6134,12 +6134,12 @@
       </c>
       <c r="N61" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -6154,7 +6154,7 @@
       </c>
       <c r="R61" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Good marks in Operation Research</t>
         </is>
       </c>
       <c r="S61" t="inlineStr">
@@ -6219,7 +6219,7 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M62" t="inlineStr">
@@ -6229,17 +6229,17 @@
       </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q62" t="inlineStr">
@@ -6249,7 +6249,7 @@
       </c>
       <c r="R62" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S62" t="inlineStr">
@@ -6314,7 +6314,7 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Average marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M63" t="inlineStr">
@@ -6339,7 +6339,7 @@
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R63" t="inlineStr">
@@ -6409,7 +6409,7 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M64" t="inlineStr">
@@ -6424,17 +6424,17 @@
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R64" t="inlineStr">
@@ -6519,12 +6519,12 @@
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q65" t="inlineStr">
@@ -6599,7 +6599,7 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M66" t="inlineStr">
@@ -6609,7 +6609,7 @@
       </c>
       <c r="N66" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O66" t="inlineStr">
@@ -6624,12 +6624,12 @@
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R66" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S66" t="inlineStr">
@@ -6694,7 +6694,7 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M67" t="inlineStr">
@@ -6704,17 +6704,17 @@
       </c>
       <c r="N67" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Good marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q67" t="inlineStr">
@@ -6724,7 +6724,7 @@
       </c>
       <c r="R67" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S67" t="inlineStr">
@@ -6789,7 +6789,7 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M68" t="inlineStr">
@@ -6799,27 +6799,27 @@
       </c>
       <c r="N68" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R68" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S68" t="inlineStr">
@@ -6884,7 +6884,7 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M69" t="inlineStr">
@@ -6894,7 +6894,7 @@
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O69" t="inlineStr">
@@ -6904,12 +6904,12 @@
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q69" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R69" t="inlineStr">
@@ -6989,17 +6989,17 @@
       </c>
       <c r="N70" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q70" t="inlineStr">
@@ -7009,7 +7009,7 @@
       </c>
       <c r="R70" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S70" t="inlineStr">
@@ -7074,7 +7074,7 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M71" t="inlineStr">
@@ -7084,27 +7084,27 @@
       </c>
       <c r="N71" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q71" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R71" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S71" t="inlineStr">
@@ -7179,7 +7179,7 @@
       </c>
       <c r="N72" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Good marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O72" t="inlineStr">
@@ -7194,7 +7194,7 @@
       </c>
       <c r="Q72" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R72" t="inlineStr">
@@ -7264,7 +7264,7 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>Poor marks in Discrete Mathematics</t>
+          <t>Average marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M73" t="inlineStr">
@@ -7274,27 +7274,27 @@
       </c>
       <c r="N73" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Poor marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q73" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R73" t="inlineStr">
         <is>
-          <t>Poor marks in Operation Research</t>
+          <t>Good marks in Operation Research</t>
         </is>
       </c>
       <c r="S73" t="inlineStr">
@@ -7359,7 +7359,7 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Poor marks in Discrete Mathematics</t>
+          <t>Average marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M74" t="inlineStr">
@@ -7369,22 +7369,22 @@
       </c>
       <c r="N74" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Good marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>Poor marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R74" t="inlineStr">
@@ -7454,7 +7454,7 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M75" t="inlineStr">
@@ -7469,7 +7469,7 @@
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Good marks in Computer Networks</t>
+          <t>Average marks in Computer Networks</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -7479,12 +7479,12 @@
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R75" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S75" t="inlineStr">
@@ -7559,17 +7559,17 @@
       </c>
       <c r="N76" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>Poor marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q76" t="inlineStr">
@@ -7579,7 +7579,7 @@
       </c>
       <c r="R76" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S76" t="inlineStr">
@@ -7664,17 +7664,17 @@
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Poor marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q77" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R77" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S77" t="inlineStr">
@@ -7739,7 +7739,7 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M78" t="inlineStr">
@@ -7749,7 +7749,7 @@
       </c>
       <c r="N78" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O78" t="inlineStr">
@@ -7764,12 +7764,12 @@
       </c>
       <c r="Q78" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R78" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S78" t="inlineStr">
@@ -7849,7 +7849,7 @@
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -7929,7 +7929,7 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
@@ -7939,7 +7939,7 @@
       </c>
       <c r="N80" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O80" t="inlineStr">
@@ -7949,17 +7949,17 @@
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R80" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S80" t="inlineStr">
@@ -8039,7 +8039,7 @@
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Poor marks in Computer Networks</t>
+          <t>Average marks in Computer Networks</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -8049,12 +8049,12 @@
       </c>
       <c r="Q81" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R81" t="inlineStr">
         <is>
-          <t>Poor marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S81" t="inlineStr">
@@ -8129,7 +8129,7 @@
       </c>
       <c r="N82" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O82" t="inlineStr">
@@ -8139,7 +8139,7 @@
       </c>
       <c r="P82" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q82" t="inlineStr">
@@ -8149,7 +8149,7 @@
       </c>
       <c r="R82" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S82" t="inlineStr">
@@ -8214,7 +8214,7 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
@@ -8239,7 +8239,7 @@
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R83" t="inlineStr">
@@ -8324,22 +8324,22 @@
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R84" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S84" t="inlineStr">
@@ -8404,7 +8404,7 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M85" t="inlineStr">
@@ -8424,17 +8424,17 @@
       </c>
       <c r="P85" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R85" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S85" t="inlineStr">
@@ -8499,7 +8499,7 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M86" t="inlineStr">
@@ -8509,22 +8509,22 @@
       </c>
       <c r="N86" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q86" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R86" t="inlineStr">
@@ -8594,7 +8594,7 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M87" t="inlineStr">
@@ -8604,27 +8604,27 @@
       </c>
       <c r="N87" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P87" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q87" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R87" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S87" t="inlineStr">
@@ -8689,7 +8689,7 @@
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M88" t="inlineStr">
@@ -8699,17 +8699,17 @@
       </c>
       <c r="N88" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q88" t="inlineStr">
@@ -8719,7 +8719,7 @@
       </c>
       <c r="R88" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S88" t="inlineStr">
@@ -8794,7 +8794,7 @@
       </c>
       <c r="N89" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Good marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O89" t="inlineStr">
@@ -8804,17 +8804,17 @@
       </c>
       <c r="P89" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q89" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R89" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S89" t="inlineStr">
@@ -8889,7 +8889,7 @@
       </c>
       <c r="N90" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O90" t="inlineStr">
@@ -8899,17 +8899,17 @@
       </c>
       <c r="P90" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q90" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R90" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S90" t="inlineStr">
@@ -8974,7 +8974,7 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M91" t="inlineStr">
@@ -8989,22 +8989,22 @@
       </c>
       <c r="O91" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P91" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q91" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R91" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S91" t="inlineStr">
@@ -9094,12 +9094,12 @@
       </c>
       <c r="Q92" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R92" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S92" t="inlineStr">
@@ -9174,7 +9174,7 @@
       </c>
       <c r="N93" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O93" t="inlineStr">
@@ -9184,7 +9184,7 @@
       </c>
       <c r="P93" t="inlineStr">
         <is>
-          <t>Poor marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q93" t="inlineStr">
@@ -9259,7 +9259,7 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>Poor marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M94" t="inlineStr">
@@ -9274,22 +9274,22 @@
       </c>
       <c r="O94" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P94" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q94" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R94" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S94" t="inlineStr">
@@ -9354,7 +9354,7 @@
       </c>
       <c r="L95" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M95" t="inlineStr">
@@ -9364,27 +9364,27 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Good marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O95" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P95" t="inlineStr">
         <is>
-          <t>Poor marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q95" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R95" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S95" t="inlineStr">
@@ -9469,17 +9469,17 @@
       </c>
       <c r="P96" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R96" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S96" t="inlineStr">
@@ -9544,7 +9544,7 @@
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Average marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M97" t="inlineStr">
@@ -9564,12 +9564,12 @@
       </c>
       <c r="P97" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q97" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R97" t="inlineStr">
@@ -9639,7 +9639,7 @@
       </c>
       <c r="L98" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M98" t="inlineStr">
@@ -9654,12 +9654,12 @@
       </c>
       <c r="O98" t="inlineStr">
         <is>
-          <t>Good marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P98" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q98" t="inlineStr">
@@ -9734,7 +9734,7 @@
       </c>
       <c r="L99" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M99" t="inlineStr">
@@ -9749,22 +9749,22 @@
       </c>
       <c r="O99" t="inlineStr">
         <is>
-          <t>Poor marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P99" t="inlineStr">
         <is>
-          <t>Poor marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q99" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R99" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Good marks in Operation Research</t>
         </is>
       </c>
       <c r="S99" t="inlineStr">
@@ -9829,7 +9829,7 @@
       </c>
       <c r="L100" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M100" t="inlineStr">
@@ -9844,7 +9844,7 @@
       </c>
       <c r="O100" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P100" t="inlineStr">
@@ -9859,7 +9859,7 @@
       </c>
       <c r="R100" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S100" t="inlineStr">
@@ -9939,22 +9939,22 @@
       </c>
       <c r="O101" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P101" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q101" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R101" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Good marks in Operation Research</t>
         </is>
       </c>
       <c r="S101" t="inlineStr">
@@ -10019,7 +10019,7 @@
       </c>
       <c r="L102" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M102" t="inlineStr">
@@ -10029,7 +10029,7 @@
       </c>
       <c r="N102" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O102" t="inlineStr">
@@ -10039,12 +10039,12 @@
       </c>
       <c r="P102" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q102" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R102" t="inlineStr">
@@ -10114,7 +10114,7 @@
       </c>
       <c r="L103" t="inlineStr">
         <is>
-          <t>Poor marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M103" t="inlineStr">
@@ -10124,27 +10124,27 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>Poor marks in Data Base Management System</t>
+          <t>Good marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O103" t="inlineStr">
         <is>
-          <t>Poor marks in Computer Networks</t>
+          <t>Average marks in Computer Networks</t>
         </is>
       </c>
       <c r="P103" t="inlineStr">
         <is>
-          <t>Poor marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
-          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R103" t="inlineStr">
         <is>
-          <t>Poor marks in Operation Research</t>
+          <t>Good marks in Operation Research</t>
         </is>
       </c>
       <c r="S103" t="inlineStr">
@@ -10209,7 +10209,7 @@
       </c>
       <c r="L104" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M104" t="inlineStr">
@@ -10219,27 +10219,27 @@
       </c>
       <c r="N104" t="inlineStr">
         <is>
-          <t>Good marks in Data Base Management System</t>
+          <t>Average marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O104" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P104" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q104" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R104" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S104" t="inlineStr">
@@ -10304,7 +10304,7 @@
       </c>
       <c r="L105" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M105" t="inlineStr">
@@ -10319,22 +10319,22 @@
       </c>
       <c r="O105" t="inlineStr">
         <is>
-          <t>Good marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P105" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q105" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R105" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S105" t="inlineStr">
@@ -10399,7 +10399,7 @@
       </c>
       <c r="L106" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M106" t="inlineStr">
@@ -10414,22 +10414,22 @@
       </c>
       <c r="O106" t="inlineStr">
         <is>
-          <t>Good marks in Computer Networks</t>
+          <t>Average marks in Computer Networks</t>
         </is>
       </c>
       <c r="P106" t="inlineStr">
         <is>
-          <t>Good marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q106" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R106" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S106" t="inlineStr">
@@ -10494,7 +10494,7 @@
       </c>
       <c r="L107" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M107" t="inlineStr">
@@ -10519,12 +10519,12 @@
       </c>
       <c r="Q107" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R107" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S107" t="inlineStr">
@@ -10604,7 +10604,7 @@
       </c>
       <c r="O108" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P108" t="inlineStr">
@@ -10684,7 +10684,7 @@
       </c>
       <c r="L109" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M109" t="inlineStr">
@@ -10694,17 +10694,17 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Good marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O109" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Poor marks in Computer Networks</t>
         </is>
       </c>
       <c r="P109" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q109" t="inlineStr">
@@ -10714,7 +10714,7 @@
       </c>
       <c r="R109" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S109" t="inlineStr">
@@ -10779,7 +10779,7 @@
       </c>
       <c r="L110" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M110" t="inlineStr">
@@ -10804,12 +10804,12 @@
       </c>
       <c r="Q110" t="inlineStr">
         <is>
-          <t>Good marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R110" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S110" t="inlineStr">
@@ -10884,27 +10884,27 @@
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Poor marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O111" t="inlineStr">
         <is>
-          <t>Average marks in Computer Networks</t>
+          <t>Good marks in Computer Networks</t>
         </is>
       </c>
       <c r="P111" t="inlineStr">
         <is>
-          <t>Poor marks in Operating System</t>
+          <t>Good marks in Operating System</t>
         </is>
       </c>
       <c r="Q111" t="inlineStr">
         <is>
-          <t>Average marks in Information Theory &amp; Coding / Computer Graphics</t>
+          <t>Poor marks in Information Theory &amp; Coding / Computer Graphics</t>
         </is>
       </c>
       <c r="R111" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S111" t="inlineStr">
@@ -10969,7 +10969,7 @@
       </c>
       <c r="L112" t="inlineStr">
         <is>
-          <t>Average marks in Discrete Mathematics</t>
+          <t>Good marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M112" t="inlineStr">
@@ -10989,7 +10989,7 @@
       </c>
       <c r="P112" t="inlineStr">
         <is>
-          <t>Poor marks in Operating System</t>
+          <t>Average marks in Operating System</t>
         </is>
       </c>
       <c r="Q112" t="inlineStr">
@@ -10999,7 +10999,7 @@
       </c>
       <c r="R112" t="inlineStr">
         <is>
-          <t>Average marks in Operation Research</t>
+          <t>Poor marks in Operation Research</t>
         </is>
       </c>
       <c r="S112" t="inlineStr">
@@ -11064,7 +11064,7 @@
       </c>
       <c r="L113" t="inlineStr">
         <is>
-          <t>Good marks in Discrete Mathematics</t>
+          <t>Poor marks in Discrete Mathematics</t>
         </is>
       </c>
       <c r="M113" t="inlineStr">
@@ -11074,7 +11074,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>Average marks in Data Base Management System</t>
+          <t>Good marks in Data Base Management System</t>
         </is>
       </c>
       <c r="O113" t="inlineStr">
@@ -11084,7 +11084,7 @@
       </c>
       <c r="P113" t="inlineStr">
         <is>
-          <t>Average marks in Operating System</t>
+          <t>Poor marks in Operating System</t>
         </is>
       </c>
       <c r="Q113" t="inlineStr">
@@ -11094,7 +11094,7 @@
       </c>
       <c r="R113" t="inlineStr">
         <is>
-          <t>Good marks in Operation Research</t>
+          <t>Average marks in Operation Research</t>
         </is>
       </c>
       <c r="S113" t="inlineStr">

</xml_diff>